<commit_message>
sesion 2 from sat
</commit_message>
<xml_diff>
--- a/DnData/D20/NJT/MYLUCK_21Camp_Zion.xlsx
+++ b/DnData/D20/NJT/MYLUCK_21Camp_Zion.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matt8\repo\mghoskins-Data\DnData\D20\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matt8\repo\mghoskins-Data\DnData\D20\NJT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80212168-3156-4B41-A23A-61CBCDED2745}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94043065-1423-49F2-95D9-8AFA6CBBDD67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{555EC10F-2DA9-4A2E-ABDF-A872F8AFBE1A}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="10">
   <si>
     <t>Number Rolled</t>
   </si>
@@ -60,6 +60,9 @@
   </si>
   <si>
     <t>Start: Fall 21 (9/18/21)</t>
+  </si>
+  <si>
+    <t>Portent:</t>
   </si>
 </sst>
 </file>
@@ -314,26 +317,41 @@
                 <c:pt idx="4">
                   <c:v>1</c:v>
                 </c:pt>
+                <c:pt idx="5">
+                  <c:v>1</c:v>
+                </c:pt>
                 <c:pt idx="6">
-                  <c:v>1</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>2</c:v>
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="16">
                   <c:v>1</c:v>
                 </c:pt>
+                <c:pt idx="17">
+                  <c:v>2</c:v>
+                </c:pt>
                 <c:pt idx="18">
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>1</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -935,26 +953,41 @@
                 <c:pt idx="4">
                   <c:v>1</c:v>
                 </c:pt>
+                <c:pt idx="5">
+                  <c:v>1</c:v>
+                </c:pt>
                 <c:pt idx="6">
-                  <c:v>1</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>2</c:v>
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="16">
                   <c:v>1</c:v>
                 </c:pt>
+                <c:pt idx="17">
+                  <c:v>2</c:v>
+                </c:pt>
                 <c:pt idx="18">
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>1</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2266,13 +2299,13 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>137160</xdr:colOff>
+      <xdr:colOff>60960</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>64770</xdr:rowOff>
+      <xdr:rowOff>129540</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>152400</xdr:colOff>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>18</xdr:row>
       <xdr:rowOff>45720</xdr:rowOff>
     </xdr:to>
@@ -2302,15 +2335,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>167640</xdr:colOff>
+      <xdr:colOff>38100</xdr:colOff>
       <xdr:row>18</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
+      <xdr:rowOff>167640</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>182880</xdr:colOff>
+      <xdr:colOff>53340</xdr:colOff>
       <xdr:row>36</xdr:row>
-      <xdr:rowOff>133350</xdr:rowOff>
+      <xdr:rowOff>148590</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2640,18 +2673,20 @@
   <dimension ref="A1:V28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="21.109375" customWidth="1"/>
     <col min="2" max="2" width="15.21875" customWidth="1"/>
+    <col min="16" max="16" width="8.88671875" customWidth="1"/>
     <col min="18" max="18" width="17.77734375" customWidth="1"/>
-    <col min="19" max="19" width="14.5546875" customWidth="1"/>
+    <col min="19" max="19" width="15.5546875" customWidth="1"/>
+    <col min="20" max="20" width="13.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -2661,11 +2696,20 @@
       <c r="C1" t="s">
         <v>3</v>
       </c>
-      <c r="Q1" s="1"/>
-      <c r="R1" s="1"/>
-      <c r="S1" s="1"/>
+      <c r="Q1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>3</v>
+      </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -2675,10 +2719,16 @@
         <v>0</v>
       </c>
       <c r="Q2" s="1"/>
-      <c r="R2" s="1"/>
+      <c r="R2" s="1">
+        <v>1</v>
+      </c>
       <c r="S2" s="1"/>
+      <c r="T2">
+        <f>S2/S22</f>
+        <v>0</v>
+      </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -2688,10 +2738,16 @@
         <v>0</v>
       </c>
       <c r="Q3" s="1"/>
-      <c r="R3" s="1"/>
+      <c r="R3" s="1">
+        <v>2</v>
+      </c>
       <c r="S3" s="1"/>
+      <c r="T3">
+        <f>S3/S22</f>
+        <v>0</v>
+      </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -2701,10 +2757,16 @@
         <v>0</v>
       </c>
       <c r="Q4" s="1"/>
-      <c r="R4" s="1"/>
+      <c r="R4" s="1">
+        <v>3</v>
+      </c>
       <c r="S4" s="1"/>
+      <c r="T4">
+        <f>S4/S22</f>
+        <v>0</v>
+      </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -2714,10 +2776,16 @@
         <v>0</v>
       </c>
       <c r="Q5" s="1"/>
-      <c r="R5" s="1"/>
+      <c r="R5" s="1">
+        <v>4</v>
+      </c>
       <c r="S5" s="1"/>
+      <c r="T5">
+        <f>S5/S22</f>
+        <v>0</v>
+      </c>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -2726,56 +2794,84 @@
       </c>
       <c r="C6" s="3">
         <f>B6/B22 * 100</f>
-        <v>11.111111111111111</v>
+        <v>5.2631578947368416</v>
       </c>
       <c r="Q6" s="1"/>
-      <c r="R6" s="1"/>
+      <c r="R6" s="1">
+        <v>5</v>
+      </c>
       <c r="S6" s="1"/>
+      <c r="T6">
+        <f>S6/S22</f>
+        <v>0</v>
+      </c>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
         <v>6</v>
       </c>
-      <c r="B7" s="2"/>
+      <c r="B7" s="2">
+        <v>1</v>
+      </c>
       <c r="C7" s="3">
         <f>B7/B22 * 100</f>
+        <v>5.2631578947368416</v>
+      </c>
+      <c r="Q7" s="1"/>
+      <c r="R7" s="1">
+        <v>6</v>
+      </c>
+      <c r="S7" s="1"/>
+      <c r="T7">
+        <f>S7/S22</f>
         <v>0</v>
       </c>
-      <c r="Q7" s="1"/>
-      <c r="R7" s="1"/>
-      <c r="S7" s="1"/>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
         <v>7</v>
       </c>
       <c r="B8" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C8" s="3">
         <f>B8/B22 * 100</f>
-        <v>11.111111111111111</v>
+        <v>10.526315789473683</v>
       </c>
       <c r="Q8" s="1"/>
-      <c r="R8" s="1"/>
-      <c r="S8" s="1"/>
+      <c r="R8" s="1">
+        <v>7</v>
+      </c>
+      <c r="S8" s="1">
+        <v>1</v>
+      </c>
+      <c r="T8">
+        <f>S8/S22</f>
+        <v>0.5</v>
+      </c>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A9" s="2">
         <v>8</v>
       </c>
       <c r="B9" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C9" s="3">
         <f>B9/B22 * 100</f>
-        <v>11.111111111111111</v>
+        <v>10.526315789473683</v>
       </c>
       <c r="Q9" s="1"/>
-      <c r="R9" s="1"/>
+      <c r="R9" s="1">
+        <v>8</v>
+      </c>
       <c r="S9" s="1"/>
+      <c r="T9">
+        <f>S9/S22</f>
+        <v>0</v>
+      </c>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A10" s="2">
         <v>9</v>
       </c>
@@ -2784,54 +2880,82 @@
       </c>
       <c r="C10" s="3">
         <f>B10/B22 * 100</f>
-        <v>11.111111111111111</v>
+        <v>5.2631578947368416</v>
       </c>
       <c r="Q10" s="1"/>
-      <c r="R10" s="1"/>
+      <c r="R10" s="1">
+        <v>9</v>
+      </c>
       <c r="S10" s="1"/>
+      <c r="T10">
+        <f>S10/S22</f>
+        <v>0</v>
+      </c>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A11" s="2">
         <v>10</v>
       </c>
       <c r="B11" s="2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C11" s="3">
         <f>B11/B22 * 100</f>
-        <v>22.222222222222221</v>
+        <v>15.789473684210526</v>
       </c>
       <c r="Q11" s="1"/>
-      <c r="R11" s="1"/>
+      <c r="R11" s="1">
+        <v>10</v>
+      </c>
       <c r="S11" s="1"/>
+      <c r="T11">
+        <f>S11/S22</f>
+        <v>0</v>
+      </c>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A12" s="2">
         <v>11</v>
       </c>
-      <c r="B12" s="2"/>
+      <c r="B12" s="2">
+        <v>1</v>
+      </c>
       <c r="C12" s="3">
         <f>B12/B22 * 100</f>
+        <v>5.2631578947368416</v>
+      </c>
+      <c r="Q12" s="1"/>
+      <c r="R12" s="1">
+        <v>11</v>
+      </c>
+      <c r="S12" s="1"/>
+      <c r="T12">
+        <f>S12/S22</f>
         <v>0</v>
       </c>
-      <c r="Q12" s="1"/>
-      <c r="R12" s="1"/>
-      <c r="S12" s="1"/>
     </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A13" s="2">
         <v>12</v>
       </c>
-      <c r="B13" s="2"/>
+      <c r="B13" s="2">
+        <v>1</v>
+      </c>
       <c r="C13" s="3">
         <f>B13/B22 * 100</f>
+        <v>5.2631578947368416</v>
+      </c>
+      <c r="Q13" s="1"/>
+      <c r="R13" s="1">
+        <v>12</v>
+      </c>
+      <c r="S13" s="1"/>
+      <c r="T13">
+        <f>S13/S22</f>
         <v>0</v>
       </c>
-      <c r="Q13" s="1"/>
-      <c r="R13" s="1"/>
-      <c r="S13" s="1"/>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A14" s="2">
         <v>13</v>
       </c>
@@ -2841,10 +2965,16 @@
         <v>0</v>
       </c>
       <c r="Q14" s="1"/>
-      <c r="R14" s="1"/>
+      <c r="R14" s="1">
+        <v>13</v>
+      </c>
       <c r="S14" s="1"/>
+      <c r="T14">
+        <f>S14/S22</f>
+        <v>0</v>
+      </c>
     </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A15" s="2">
         <v>14</v>
       </c>
@@ -2854,21 +2984,35 @@
         <v>0</v>
       </c>
       <c r="Q15" s="1"/>
-      <c r="R15" s="1"/>
+      <c r="R15" s="1">
+        <v>14</v>
+      </c>
       <c r="S15" s="1"/>
+      <c r="T15">
+        <f>S15/S22</f>
+        <v>0</v>
+      </c>
     </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A16" s="2">
         <v>15</v>
       </c>
-      <c r="B16" s="2"/>
+      <c r="B16" s="2">
+        <v>1</v>
+      </c>
       <c r="C16" s="3">
         <f>B16/B22 * 100</f>
+        <v>5.2631578947368416</v>
+      </c>
+      <c r="Q16" s="1"/>
+      <c r="R16" s="1">
+        <v>15</v>
+      </c>
+      <c r="S16" s="1"/>
+      <c r="T16">
+        <f>S16/S22</f>
         <v>0</v>
       </c>
-      <c r="Q16" s="1"/>
-      <c r="R16" s="1"/>
-      <c r="S16" s="1"/>
     </row>
     <row r="17" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A17" s="2">
@@ -2880,8 +3024,14 @@
         <v>0</v>
       </c>
       <c r="Q17" s="1"/>
-      <c r="R17" s="1"/>
+      <c r="R17" s="1">
+        <v>16</v>
+      </c>
       <c r="S17" s="1"/>
+      <c r="T17">
+        <f>S17/S22</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="18" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A18" s="2">
@@ -2892,24 +3042,38 @@
       </c>
       <c r="C18" s="3">
         <f>B18/B22 * 100</f>
-        <v>11.111111111111111</v>
+        <v>5.2631578947368416</v>
       </c>
       <c r="Q18" s="1"/>
-      <c r="R18" s="1"/>
+      <c r="R18" s="1">
+        <v>17</v>
+      </c>
       <c r="S18" s="1"/>
+      <c r="T18">
+        <f>S18/S22</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="19" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A19" s="2">
         <v>18</v>
       </c>
-      <c r="B19" s="2"/>
+      <c r="B19" s="2">
+        <v>2</v>
+      </c>
       <c r="C19" s="3">
         <f>B19/B22 * 100</f>
+        <v>10.526315789473683</v>
+      </c>
+      <c r="Q19" s="1"/>
+      <c r="R19" s="1">
+        <v>18</v>
+      </c>
+      <c r="S19" s="1"/>
+      <c r="T19">
+        <f>S19/S22</f>
         <v>0</v>
       </c>
-      <c r="Q19" s="1"/>
-      <c r="R19" s="1"/>
-      <c r="S19" s="1"/>
       <c r="V19" t="s">
         <v>1</v>
       </c>
@@ -2923,26 +3087,40 @@
       </c>
       <c r="C20" s="3">
         <f>B20/B22 * 100</f>
-        <v>11.111111111111111</v>
+        <v>5.2631578947368416</v>
       </c>
       <c r="Q20" s="1"/>
-      <c r="R20" s="1"/>
+      <c r="R20" s="1">
+        <v>19</v>
+      </c>
       <c r="S20" s="1"/>
+      <c r="T20">
+        <f>S20/S22</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="21" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A21" s="2">
         <v>20</v>
       </c>
       <c r="B21" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C21" s="3">
         <f>B21/B22 * 100</f>
-        <v>11.111111111111111</v>
+        <v>10.526315789473683</v>
       </c>
       <c r="Q21" s="1"/>
-      <c r="R21" s="1"/>
-      <c r="S21" s="1"/>
+      <c r="R21" s="1">
+        <v>20</v>
+      </c>
+      <c r="S21" s="1">
+        <v>1</v>
+      </c>
+      <c r="T21">
+        <f>S21/S22</f>
+        <v>0.5</v>
+      </c>
     </row>
     <row r="22" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
@@ -2950,7 +3128,11 @@
       </c>
       <c r="B22">
         <f>SUM(B2:B21)</f>
-        <v>9</v>
+        <v>19</v>
+      </c>
+      <c r="S22">
+        <f>SUM(S2:S21)</f>
+        <v>2</v>
       </c>
     </row>
     <row r="23" spans="1:22" x14ac:dyDescent="0.3">
@@ -2962,11 +3144,11 @@
       </c>
       <c r="B24">
         <f>SUM(B2:B11)</f>
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C24" s="3">
         <f>SUM(C2:C11)</f>
-        <v>66.666666666666657</v>
+        <v>52.631578947368418</v>
       </c>
     </row>
     <row r="25" spans="1:22" x14ac:dyDescent="0.3">
@@ -2975,11 +3157,11 @@
       </c>
       <c r="B25">
         <f>SUM(B12:B21)</f>
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="C25" s="3">
         <f>SUM(C12:C21)</f>
-        <v>33.333333333333329</v>
+        <v>47.368421052631575</v>
       </c>
     </row>
     <row r="27" spans="1:22" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Close njt camp 1
</commit_message>
<xml_diff>
--- a/DnData/D20/NJT/MYLUCK_21Camp_Zion.xlsx
+++ b/DnData/D20/NJT/MYLUCK_21Camp_Zion.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matt8\repo\mghoskins-Data\DnData\D20\NJT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E9078E4-18A4-467B-95BD-653E867F4FB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9466D848-A2FA-46AA-8349-6802B291225B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{555EC10F-2DA9-4A2E-ABDF-A872F8AFBE1A}"/>
   </bookViews>
@@ -723,7 +723,7 @@
             </a:r>
             <a:r>
               <a:rPr lang="en-US" baseline="0"/>
-              <a:t> (2)</a:t>
+              <a:t> (1)</a:t>
             </a:r>
             <a:r>
               <a:rPr lang="en-US"/>
@@ -2715,7 +2715,7 @@
   <dimension ref="A1:V28"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>